<commit_message>
MOM, Updated User stories
</commit_message>
<xml_diff>
--- a/Process/Timesheet/MOM.xlsx
+++ b/Process/Timesheet/MOM.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25207"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6CF4AA3A-DF42-4D1A-9DC4-025DD50F36EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="105" documentId="8_{6CF4AA3A-DF42-4D1A-9DC4-025DD50F36EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F4858B4-1ACF-436A-8F58-413B7EAE94D2}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="11-04-2021" sheetId="1" r:id="rId1"/>
+    <sheet name="11-04-2022" sheetId="1" r:id="rId1"/>
+    <sheet name="12-04-2022" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="27">
   <si>
     <t>MOM</t>
   </si>
@@ -60,6 +61,54 @@
   </si>
   <si>
     <t>Start developing the Data Model</t>
+  </si>
+  <si>
+    <t>Remove Logo in Header</t>
+  </si>
+  <si>
+    <t>Don't Allow Public to Comment on any post in home page before login (Even don't allow the public to enter something in textbox)</t>
+  </si>
+  <si>
+    <t>Remove Forgot Password Checkbox in Forgot Password page</t>
+  </si>
+  <si>
+    <t>Correct All Alignment problem</t>
+  </si>
+  <si>
+    <t>Remove Remember Me Checkbox in Requester login page</t>
+  </si>
+  <si>
+    <t>If Requester Enter Any comment on any post it shows "me" (Avoid Requester name) and then what comment he gave</t>
+  </si>
+  <si>
+    <t>Correct the Breadcrumps in Requester's my award page</t>
+  </si>
+  <si>
+    <t>Remove Filter Retain Functionality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remove ACE ID dropdown box in Add an request page (instead use name or username) </t>
+  </si>
+  <si>
+    <t>Remove Preview Functionality in awardee preview in requester page</t>
+  </si>
+  <si>
+    <t>rejection reason box have only close button(remove yes no )</t>
+  </si>
+  <si>
+    <t>Remove Disable functionality in Dashboard Department filter</t>
+  </si>
+  <si>
+    <t>Use Stacked bar in dashboard</t>
+  </si>
+  <si>
+    <t>map the designation and department in data model</t>
+  </si>
+  <si>
+    <t>Remove Approver table in data model (refinment)</t>
+  </si>
+  <si>
+    <t>Start developing Physical model of data model</t>
   </si>
 </sst>
 </file>
@@ -89,7 +138,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -136,11 +185,57 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -152,6 +247,33 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -470,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C4:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -549,4 +671,279 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31E87B47-25EA-456B-9956-B1E6D165DD22}">
+  <dimension ref="B5:E38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="115.85546875" customWidth="1"/>
+    <col min="4" max="4" width="37.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:5">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="2:5">
+      <c r="B6" s="1"/>
+      <c r="C6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="2:5">
+      <c r="B7" s="1"/>
+      <c r="C7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="2:5">
+      <c r="B8" s="1"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="2:5">
+      <c r="B9" s="1"/>
+      <c r="C9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="2:5">
+      <c r="B10" s="1"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="2:5">
+      <c r="B11" s="1"/>
+      <c r="C11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="2:5">
+      <c r="B12" s="1"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="2:5">
+      <c r="B13" s="1"/>
+      <c r="C13" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="2:5">
+      <c r="B14" s="1"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="2:5">
+      <c r="C15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5">
+      <c r="C16" s="5"/>
+      <c r="D16" s="9"/>
+    </row>
+    <row r="17" spans="3:4">
+      <c r="C17" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4">
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+    </row>
+    <row r="19" spans="3:4">
+      <c r="C19" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="5"/>
+    </row>
+    <row r="20" spans="3:4">
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+    </row>
+    <row r="21" spans="3:4">
+      <c r="C21" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4">
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+    </row>
+    <row r="23" spans="3:4">
+      <c r="C23" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="3:4">
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+    </row>
+    <row r="25" spans="3:4">
+      <c r="C25" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="3:4">
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+    </row>
+    <row r="27" spans="3:4">
+      <c r="C27" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="3:4">
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+    </row>
+    <row r="29" spans="3:4">
+      <c r="C29" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="3:4">
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+    </row>
+    <row r="31" spans="3:4">
+      <c r="C31" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="3:4">
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+    </row>
+    <row r="33" spans="3:4">
+      <c r="C33" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="3:4">
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+    </row>
+    <row r="35" spans="3:4">
+      <c r="C35" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="3:4">
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+    </row>
+    <row r="37" spans="3:4">
+      <c r="C37" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="3:4">
+      <c r="C38" s="5"/>
+      <c r="D38" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="32">
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Time Sheet and MOM
</commit_message>
<xml_diff>
--- a/Process/Timesheet/MOM.xlsx
+++ b/Process/Timesheet/MOM.xlsx
@@ -3,14 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25217"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C368506-4729-40E6-98E4-FDFD24B36572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="52" documentId="8_{2F185AB4-E681-4846-9AA3-9DEB81962099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53AD5B2E-CAD6-4881-A53D-5FC110D59701}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="11-04-2022" sheetId="1" r:id="rId1"/>
     <sheet name="12-04-2022" sheetId="2" r:id="rId2"/>
     <sheet name="13-04-2022" sheetId="3" r:id="rId3"/>
+    <sheet name="20-04-2022" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="46">
   <si>
     <t>MOM</t>
   </si>
@@ -115,6 +116,9 @@
     <t>Spelling corrections in  wire frame</t>
   </si>
   <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
     <t>Alignments in wire frame</t>
   </si>
   <si>
@@ -140,6 +144,30 @@
   </si>
   <si>
     <t>Refine the operations in data model</t>
+  </si>
+  <si>
+    <t>Change datatype of the AddedBy, UpdatedBy Attributes in Award Request Table in DataModel</t>
+  </si>
+  <si>
+    <t>Spelling Correction - "Designation"</t>
+  </si>
+  <si>
+    <t>Operations in datamodel must contain Input and Output</t>
+  </si>
+  <si>
+    <t>Change FilterByAward(Award) into FilterByAward(Award type)</t>
+  </si>
+  <si>
+    <t>Naming convention - View Comments (plural)</t>
+  </si>
+  <si>
+    <t>Don't use remove functionality in status page, instead use disable functionality</t>
+  </si>
+  <si>
+    <t>Analyse the differece between GetAwardRequest and ViewPost</t>
+  </si>
+  <si>
+    <t>Add Login and Logout operations in datamodel</t>
   </si>
 </sst>
 </file>
@@ -155,7 +183,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -168,8 +196,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -284,11 +318,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -334,6 +381,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -737,8 +793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31E87B47-25EA-456B-9956-B1E6D165DD22}">
   <dimension ref="B5:E38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:D26"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1012,8 +1068,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8305E1F2-D22A-4DC8-881C-61A81FB591C3}">
   <dimension ref="E9:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14:E15"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9:F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1022,7 +1078,7 @@
     <col min="6" max="6" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="9" spans="5:6">
+    <row r="9" spans="5:8">
       <c r="E9" s="2" t="s">
         <v>0</v>
       </c>
@@ -1030,7 +1086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="5:6">
+    <row r="10" spans="5:8">
       <c r="E10" s="6" t="s">
         <v>27</v>
       </c>
@@ -1038,37 +1094,40 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="5:6">
+    <row r="11" spans="5:8">
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
-    </row>
-    <row r="12" spans="5:6">
+      <c r="H11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="5:8">
       <c r="E12" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="5:6">
+    <row r="13" spans="5:8">
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
     </row>
-    <row r="14" spans="5:6">
+    <row r="14" spans="5:8">
       <c r="E14" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="5:6">
+    <row r="15" spans="5:8">
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
     </row>
-    <row r="16" spans="5:6">
+    <row r="16" spans="5:8">
       <c r="E16" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>3</v>
@@ -1080,7 +1139,7 @@
     </row>
     <row r="18" spans="5:10">
       <c r="E18" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F18" s="11" t="s">
         <v>3</v>
@@ -1092,7 +1151,7 @@
     </row>
     <row r="20" spans="5:10">
       <c r="E20" s="11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F20" s="12" t="s">
         <v>3</v>
@@ -1104,7 +1163,7 @@
     </row>
     <row r="22" spans="5:10">
       <c r="E22" s="11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F22" s="11" t="s">
         <v>3</v>
@@ -1116,10 +1175,10 @@
     </row>
     <row r="24" spans="5:10">
       <c r="E24" s="11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="5:10">
@@ -1128,7 +1187,7 @@
     </row>
     <row r="26" spans="5:10">
       <c r="E26" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F26" s="11" t="s">
         <v>3</v>
@@ -1164,4 +1223,155 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{145DE6EF-A0C8-42DE-84D5-5522946F94F0}">
+  <dimension ref="E6:F24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9:E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="5" max="5" width="88.5703125" customWidth="1"/>
+    <col min="6" max="6" width="27.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="5:6">
+      <c r="E6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="5:6">
+      <c r="E7" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="5:6">
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" spans="5:6">
+      <c r="E9" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="5:6">
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" spans="5:6">
+      <c r="E11" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="5:6">
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" spans="5:6">
+      <c r="E13" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="5:6">
+      <c r="E14" s="7"/>
+      <c r="F14" s="10"/>
+    </row>
+    <row r="15" spans="5:6">
+      <c r="E15" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="5:6">
+      <c r="E16" s="9"/>
+      <c r="F16" s="11"/>
+    </row>
+    <row r="17" spans="5:6">
+      <c r="E17" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="5:6">
+      <c r="E18" s="19"/>
+      <c r="F18" s="13"/>
+    </row>
+    <row r="19" spans="5:6">
+      <c r="E19" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="5:6">
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+    </row>
+    <row r="21" spans="5:6">
+      <c r="E21" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="5:6">
+      <c r="E22" s="17"/>
+      <c r="F22" s="11"/>
+    </row>
+    <row r="23" spans="5:6">
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+    </row>
+    <row r="24" spans="5:6">
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="18">
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
MOM and System Architecture
</commit_message>
<xml_diff>
--- a/Process/Timesheet/MOM.xlsx
+++ b/Process/Timesheet/MOM.xlsx
@@ -3,15 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25217"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="52" documentId="8_{2F185AB4-E681-4846-9AA3-9DEB81962099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53AD5B2E-CAD6-4881-A53D-5FC110D59701}"/>
+  <xr:revisionPtr revIDLastSave="95" documentId="8_{2F185AB4-E681-4846-9AA3-9DEB81962099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{92AF9088-66D3-4AC2-B454-2963363DEA1D}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="11-04-2022" sheetId="1" r:id="rId1"/>
     <sheet name="12-04-2022" sheetId="2" r:id="rId2"/>
     <sheet name="13-04-2022" sheetId="3" r:id="rId3"/>
     <sheet name="20-04-2022" sheetId="4" r:id="rId4"/>
+    <sheet name="21-04-2022" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="54">
   <si>
     <t>MOM</t>
   </si>
@@ -161,13 +162,37 @@
     <t>Naming convention - View Comments (plural)</t>
   </si>
   <si>
-    <t>Don't use remove functionality in status page, instead use disable functionality</t>
+    <t>Don't use remove functionality , instead use disable functionality</t>
   </si>
   <si>
     <t>Analyse the differece between GetAwardRequest and ViewPost</t>
   </si>
   <si>
     <t>Add Login and Logout operations in datamodel</t>
+  </si>
+  <si>
+    <t>Need one more Attribute in both Organisation and Department entity (Operation for getting list of departments under one specific organisation)</t>
+  </si>
+  <si>
+    <t>Multiple  filters simultaneously</t>
+  </si>
+  <si>
+    <t>GetByStatus , PostView redundancy</t>
+  </si>
+  <si>
+    <t>Naming convention - Award Request become Award and Award becomes Award Type</t>
+  </si>
+  <si>
+    <t>Write operation in Status Entity</t>
+  </si>
+  <si>
+    <t>Need Designation ID, Department ID, ACE ID in Employee Entity</t>
+  </si>
+  <si>
+    <t>Logout's  input and output  method</t>
+  </si>
+  <si>
+    <t>Pass objects instead of IDs</t>
   </si>
 </sst>
 </file>
@@ -203,7 +228,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -331,11 +356,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -350,22 +393,14 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -374,7 +409,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -391,6 +435,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -793,7 +852,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31E87B47-25EA-456B-9956-B1E6D165DD22}">
   <dimension ref="B5:E38"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -821,212 +880,234 @@
     </row>
     <row r="7" spans="2:5">
       <c r="B7" s="1"/>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="8" t="s">
         <v>3</v>
       </c>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="2:5">
       <c r="B8" s="1"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="2:5">
       <c r="B9" s="1"/>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="8" t="s">
         <v>3</v>
       </c>
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="2:5">
       <c r="B10" s="1"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="2:5">
       <c r="B11" s="1"/>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="8" t="s">
         <v>3</v>
       </c>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" s="1"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="10"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="15"/>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="2:5">
       <c r="B13" s="1"/>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="7" t="s">
         <v>3</v>
       </c>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="2:5">
       <c r="B14" s="1"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="11"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="7"/>
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="2:5">
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="10" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="16" spans="2:5">
-      <c r="C16" s="11"/>
-      <c r="D16" s="13"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="11"/>
     </row>
     <row r="17" spans="3:4">
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="18" spans="3:4">
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
     </row>
     <row r="19" spans="3:4">
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="11"/>
+      <c r="D19" s="7"/>
     </row>
     <row r="20" spans="3:4">
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
     </row>
     <row r="21" spans="3:4">
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D21" s="7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="22" spans="3:4">
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
     </row>
     <row r="23" spans="3:4">
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="11" t="s">
+      <c r="D23" s="7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="24" spans="3:4">
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
     </row>
     <row r="25" spans="3:4">
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D25" s="11" t="s">
+      <c r="D25" s="7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="26" spans="3:4">
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
     </row>
     <row r="27" spans="3:4">
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D27" s="11" t="s">
+      <c r="D27" s="7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="28" spans="3:4">
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
     </row>
     <row r="29" spans="3:4">
-      <c r="C29" s="11" t="s">
+      <c r="C29" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D29" s="11" t="s">
+      <c r="D29" s="7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="30" spans="3:4">
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
     </row>
     <row r="31" spans="3:4">
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D31" s="11" t="s">
+      <c r="D31" s="7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="32" spans="3:4">
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
     </row>
     <row r="33" spans="3:4">
-      <c r="C33" s="11" t="s">
+      <c r="C33" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D33" s="11" t="s">
+      <c r="D33" s="7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="34" spans="3:4">
-      <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
     </row>
     <row r="35" spans="3:4">
-      <c r="C35" s="11" t="s">
+      <c r="C35" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D35" s="11" t="s">
+      <c r="D35" s="7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="36" spans="3:4">
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
     </row>
     <row r="37" spans="3:4">
-      <c r="C37" s="11" t="s">
+      <c r="C37" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D37" s="14" t="s">
+      <c r="D37" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="38" spans="3:4">
-      <c r="C38" s="11"/>
-      <c r="D38" s="14"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
     <mergeCell ref="C35:C36"/>
     <mergeCell ref="D35:D36"/>
     <mergeCell ref="C37:C38"/>
@@ -1037,28 +1118,6 @@
     <mergeCell ref="D31:D32"/>
     <mergeCell ref="C33:C34"/>
     <mergeCell ref="D33:D34"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="D13:D14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1087,121 +1146,129 @@
       </c>
     </row>
     <row r="10" spans="5:8">
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="5:8">
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
       <c r="H11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="12" spans="5:8">
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="5:8">
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
     </row>
     <row r="14" spans="5:8">
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="15" spans="5:8">
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
     </row>
     <row r="16" spans="5:8">
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="17" spans="5:10">
-      <c r="E17" s="7"/>
-      <c r="F17" s="10"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="15"/>
     </row>
     <row r="18" spans="5:10">
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="F18" s="7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="19" spans="5:10">
-      <c r="E19" s="9"/>
-      <c r="F19" s="11"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="7"/>
     </row>
     <row r="20" spans="5:10">
-      <c r="E20" s="11" t="s">
+      <c r="E20" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="F20" s="12" t="s">
+      <c r="F20" s="10" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="21" spans="5:10">
-      <c r="E21" s="11"/>
-      <c r="F21" s="13"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="11"/>
     </row>
     <row r="22" spans="5:10">
-      <c r="E22" s="11" t="s">
+      <c r="E22" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F22" s="11" t="s">
+      <c r="F22" s="7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="23" spans="5:10">
-      <c r="E23" s="6"/>
-      <c r="F23" s="11"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="7"/>
     </row>
     <row r="24" spans="5:10">
-      <c r="E24" s="11" t="s">
+      <c r="E24" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="F24" s="15" t="s">
+      <c r="F24" s="16" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="25" spans="5:10">
-      <c r="E25" s="11"/>
-      <c r="F25" s="16"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="17"/>
     </row>
     <row r="26" spans="5:10">
-      <c r="E26" s="7" t="s">
+      <c r="E26" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="F26" s="11" t="s">
+      <c r="F26" s="7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="27" spans="5:10">
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
     </row>
     <row r="30" spans="5:10">
       <c r="J30" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
     <mergeCell ref="E26:E27"/>
     <mergeCell ref="F26:F27"/>
     <mergeCell ref="E18:E19"/>
@@ -1212,14 +1279,6 @@
     <mergeCell ref="F22:F23"/>
     <mergeCell ref="F24:F25"/>
     <mergeCell ref="E24:E25"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1229,8 +1288,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{145DE6EF-A0C8-42DE-84D5-5522946F94F0}">
   <dimension ref="E6:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9:E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1248,129 +1307,282 @@
       </c>
     </row>
     <row r="7" spans="5:6">
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="5:6">
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
     </row>
     <row r="9" spans="5:6">
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="5:6">
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
     </row>
     <row r="11" spans="5:6">
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="12" spans="5:6">
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
     </row>
     <row r="13" spans="5:6">
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="14" spans="5:6">
-      <c r="E14" s="7"/>
-      <c r="F14" s="10"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="15"/>
     </row>
     <row r="15" spans="5:6">
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="F15" s="11" t="s">
+      <c r="F15" s="7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="16" spans="5:6">
-      <c r="E16" s="9"/>
-      <c r="F16" s="11"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="7"/>
     </row>
     <row r="17" spans="5:6">
-      <c r="E17" s="19" t="s">
+      <c r="E17" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="F17" s="12" t="s">
+      <c r="F17" s="10" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="18" spans="5:6">
-      <c r="E18" s="19"/>
-      <c r="F18" s="13"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="11"/>
     </row>
     <row r="19" spans="5:6">
-      <c r="E19" s="11" t="s">
+      <c r="E19" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="F19" s="7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="20" spans="5:6">
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
     </row>
     <row r="21" spans="5:6">
-      <c r="E21" s="17" t="s">
+      <c r="E21" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="F21" s="11" t="s">
+      <c r="F21" s="7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="22" spans="5:6">
-      <c r="E22" s="17"/>
-      <c r="F22" s="11"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="7"/>
     </row>
     <row r="23" spans="5:6">
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
     </row>
     <row r="24" spans="5:6">
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="F17:F18"/>
     <mergeCell ref="E19:E20"/>
     <mergeCell ref="F19:F20"/>
     <mergeCell ref="E21:E22"/>
     <mergeCell ref="F21:F22"/>
     <mergeCell ref="E23:E24"/>
     <mergeCell ref="F23:F24"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A49CF707-D61D-404F-B68B-0D7CFE336593}">
+  <dimension ref="D8:F26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15:E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="4.5703125" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="5" max="5" width="123.5703125" customWidth="1"/>
+    <col min="6" max="6" width="26.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="8" spans="4:6">
+      <c r="E8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="4:6">
+      <c r="D9" s="6"/>
+      <c r="E9" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="4:6">
+      <c r="D10" s="6"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+    </row>
+    <row r="11" spans="4:6">
+      <c r="E11" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="4:6">
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+    </row>
+    <row r="13" spans="4:6">
+      <c r="E13" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="4:6">
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+    </row>
+    <row r="15" spans="4:6">
+      <c r="E15" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="4:6">
+      <c r="E16" s="12"/>
+      <c r="F16" s="15"/>
+    </row>
+    <row r="17" spans="5:6">
+      <c r="E17" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="5:6">
+      <c r="E18" s="14"/>
+      <c r="F18" s="8"/>
+    </row>
+    <row r="19" spans="5:6">
+      <c r="E19" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="5:6">
+      <c r="E20" s="24"/>
+      <c r="F20" s="25"/>
+    </row>
+    <row r="21" spans="5:6">
+      <c r="E21" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F21" s="16"/>
+    </row>
+    <row r="22" spans="5:6">
+      <c r="E22" s="15"/>
+      <c r="F22" s="23"/>
+    </row>
+    <row r="23" spans="5:6">
+      <c r="E23" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="5:6">
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+    </row>
+    <row r="25" spans="5:6">
+      <c r="E25" s="21"/>
+      <c r="F25" s="22"/>
+    </row>
+    <row r="26" spans="5:6">
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+    </row>
+  </sheetData>
+  <mergeCells count="18">
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
     <mergeCell ref="E13:E14"/>
     <mergeCell ref="F13:F14"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:F24"/>
     <mergeCell ref="E15:E16"/>
     <mergeCell ref="F15:F16"/>
     <mergeCell ref="E17:E18"/>
     <mergeCell ref="F17:F18"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>